<commit_message>
Added support for e-fuels and bio fuels differentiation Updated the calculator with finalized provisions of ETS and currently most likely landing zone of Refuel Aviation and ETD.
</commit_message>
<xml_diff>
--- a/data/simulationDefaults.xlsx
+++ b/data/simulationDefaults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7662449D-0E2F-4640-AA25-96FCB77FC471}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3157324B-0622-4FE7-8A51-4F403B013162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" xr2:uid="{5264FDAF-AE4F-4527-958C-6000D3E71A30}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{5264FDAF-AE4F-4527-958C-6000D3E71A30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="23">
   <si>
     <t>ADEP_REGION</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>RFNBO_PRICE</t>
+  </si>
+  <si>
+    <t>RFNBO_BLENDING</t>
+  </si>
+  <si>
+    <t>BIO_TAXRATE</t>
+  </si>
+  <si>
+    <t>RFNBO_TAXRATE</t>
+  </si>
+  <si>
+    <t>EXTRAEU_ETS</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -91,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,30 +453,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82F05FF-7451-4721-9C0C-DE24F786DBB2}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -471,31 +501,46 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -512,31 +557,46 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>1.075</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>25</v>
+        <v>0.81</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2">
+        <v>33</v>
+      </c>
+      <c r="O2">
         <v>90</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -550,35 +610,50 @@
         <f>E2-0.03</f>
         <v>3.6300000000000003</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>0.81</v>
-      </c>
-      <c r="H3">
-        <v>2.15</v>
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>50</v>
+        <v>0.81</v>
       </c>
       <c r="J3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
       </c>
       <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -596,31 +671,46 @@
         <v>2.5</v>
       </c>
       <c r="G4">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>3.2249999999999996</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>75</v>
+        <v>0.81</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4">
         <v>110</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -638,31 +728,46 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>4.3</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5">
+        <v>100</v>
+      </c>
+      <c r="O5">
         <v>120</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -680,31 +785,46 @@
         <v>3.5</v>
       </c>
       <c r="G6">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>5.375</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J6">
+        <v>6.14</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <v>100</v>
+      </c>
+      <c r="O6">
         <v>130</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -722,31 +842,46 @@
         <v>4</v>
       </c>
       <c r="G7">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>6.45</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J7">
+        <v>6.14</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7">
         <v>140</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -760,35 +895,50 @@
         <f t="shared" si="0"/>
         <v>3.4800000000000013</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>5</v>
       </c>
       <c r="G8">
-        <v>0.81</v>
-      </c>
-      <c r="H8">
-        <v>7.5250000000000004</v>
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.7</v>
       </c>
       <c r="I8">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J8">
+        <v>6.14</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8">
         <v>150</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -803,34 +953,49 @@
         <v>3.4500000000000015</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H9">
-        <v>8.6</v>
+        <v>1.3</v>
       </c>
       <c r="I9">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J9">
+        <v>6.14</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
+      <c r="O9">
         <v>160</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -845,34 +1010,49 @@
         <v>3.4200000000000017</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H10">
-        <v>9.6749999999999989</v>
+        <v>1.6</v>
       </c>
       <c r="I10">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J10">
+        <v>6.14</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10">
         <v>170</v>
       </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -887,34 +1067,49 @@
         <v>3.3900000000000019</v>
       </c>
       <c r="F11">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>10.749999999999998</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J11">
+        <v>12.28</v>
+      </c>
+      <c r="K11">
+        <v>6.15</v>
+      </c>
+      <c r="L11">
+        <v>0.17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
         <v>180</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -929,34 +1124,49 @@
         <v>3.3600000000000021</v>
       </c>
       <c r="F12">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G12">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>10.75</v>
+        <v>3.5</v>
       </c>
       <c r="I12">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J12">
+        <v>12.28</v>
+      </c>
+      <c r="K12">
+        <v>6.15</v>
+      </c>
+      <c r="L12">
+        <v>0.17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
         <v>190</v>
       </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -970,35 +1180,50 @@
         <f t="shared" si="0"/>
         <v>3.3300000000000023</v>
       </c>
-      <c r="F13">
-        <v>20</v>
+      <c r="F13" s="2">
+        <v>15</v>
       </c>
       <c r="G13">
-        <v>0.81</v>
-      </c>
-      <c r="H13">
-        <v>10.75</v>
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J13">
+        <v>12.28</v>
+      </c>
+      <c r="K13">
+        <v>6.15</v>
+      </c>
+      <c r="L13">
+        <v>0.17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="O13">
         <v>200</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -1013,34 +1238,49 @@
         <v>3.3000000000000025</v>
       </c>
       <c r="F14">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G14">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H14">
-        <v>10.75</v>
+        <v>5.5</v>
       </c>
       <c r="I14">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J14">
+        <v>12.28</v>
+      </c>
+      <c r="K14">
+        <v>6.15</v>
+      </c>
+      <c r="L14">
+        <v>0.17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14">
+        <v>100</v>
+      </c>
+      <c r="O14">
         <v>200</v>
       </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -1055,34 +1295,49 @@
         <v>3.2700000000000027</v>
       </c>
       <c r="F15">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G15">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <v>10.75</v>
+        <v>6</v>
       </c>
       <c r="I15">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J15">
+        <v>12.28</v>
+      </c>
+      <c r="K15">
+        <v>6.15</v>
+      </c>
+      <c r="L15">
+        <v>0.17</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15">
         <v>200</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>16</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -1097,34 +1352,49 @@
         <v>3.2400000000000029</v>
       </c>
       <c r="F16">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G16">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>10.75</v>
+        <v>6.5</v>
       </c>
       <c r="I16">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J16">
+        <v>12.28</v>
+      </c>
+      <c r="K16">
+        <v>6.15</v>
+      </c>
+      <c r="L16">
+        <v>0.17</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+      <c r="O16">
         <v>200</v>
       </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -1139,34 +1409,49 @@
         <v>3.2100000000000031</v>
       </c>
       <c r="F17">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G17">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H17">
-        <v>10.75</v>
+        <v>7</v>
       </c>
       <c r="I17">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J17">
+        <v>12.28</v>
+      </c>
+      <c r="K17">
+        <v>6.15</v>
+      </c>
+      <c r="L17">
+        <v>0.17</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
+      <c r="O17">
         <v>200</v>
       </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -1180,35 +1465,50 @@
         <f t="shared" si="0"/>
         <v>3.1800000000000033</v>
       </c>
-      <c r="F18">
-        <v>32</v>
+      <c r="F18" s="2">
+        <v>24</v>
       </c>
       <c r="G18">
-        <v>0.81</v>
-      </c>
-      <c r="H18">
-        <v>10.75</v>
+        <v>5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>8</v>
       </c>
       <c r="I18">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J18">
+        <v>12.28</v>
+      </c>
+      <c r="K18">
+        <v>6.15</v>
+      </c>
+      <c r="L18">
+        <v>0.17</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18">
         <v>200</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>16</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -1223,34 +1523,49 @@
         <v>3.1500000000000035</v>
       </c>
       <c r="F19">
-        <v>35</v>
+        <v>24.5</v>
       </c>
       <c r="G19">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>10.75</v>
+        <v>8.5</v>
       </c>
       <c r="I19">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J19">
+        <v>12.28</v>
+      </c>
+      <c r="K19">
+        <v>6.15</v>
+      </c>
+      <c r="L19">
+        <v>0.17</v>
+      </c>
+      <c r="M19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19">
         <v>200</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -1265,34 +1580,49 @@
         <v>3.1200000000000037</v>
       </c>
       <c r="F20">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="G20">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>10.75</v>
+        <v>9</v>
       </c>
       <c r="I20">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J20">
+        <v>12.28</v>
+      </c>
+      <c r="K20">
+        <v>6.15</v>
+      </c>
+      <c r="L20">
+        <v>0.17</v>
+      </c>
+      <c r="M20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20">
+        <v>100</v>
+      </c>
+      <c r="O20">
         <v>200</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>16</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -1307,34 +1637,49 @@
         <v>3.0900000000000039</v>
       </c>
       <c r="F21">
-        <v>41</v>
+        <v>25.5</v>
       </c>
       <c r="G21">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H21">
-        <v>10.75</v>
+        <v>9.5</v>
       </c>
       <c r="I21">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J21">
+        <v>12.28</v>
+      </c>
+      <c r="K21">
+        <v>6.15</v>
+      </c>
+      <c r="L21">
+        <v>0.17</v>
+      </c>
+      <c r="M21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21">
+        <v>100</v>
+      </c>
+      <c r="O21">
         <v>200</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>16</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>16</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1349,34 +1694,49 @@
         <v>3.0600000000000041</v>
       </c>
       <c r="F22">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G22">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>10.75</v>
+        <v>10</v>
       </c>
       <c r="I22">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J22">
+        <v>12.28</v>
+      </c>
+      <c r="K22">
+        <v>6.15</v>
+      </c>
+      <c r="L22">
+        <v>0.17</v>
+      </c>
+      <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
+      </c>
+      <c r="O22">
         <v>200</v>
       </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>16</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1390,35 +1750,50 @@
         <f t="shared" si="0"/>
         <v>3.0300000000000042</v>
       </c>
-      <c r="F23">
-        <v>47</v>
+      <c r="F23" s="2">
+        <v>27</v>
       </c>
       <c r="G23">
-        <v>0.81</v>
-      </c>
-      <c r="H23">
-        <v>10.75</v>
+        <v>5</v>
+      </c>
+      <c r="H23" s="2">
+        <v>11</v>
       </c>
       <c r="I23">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J23">
+        <v>12.28</v>
+      </c>
+      <c r="K23">
+        <v>6.15</v>
+      </c>
+      <c r="L23">
+        <v>0.17</v>
+      </c>
+      <c r="M23" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23">
         <v>200</v>
       </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
-        <v>16</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1433,34 +1808,49 @@
         <v>3.0000000000000044</v>
       </c>
       <c r="F24">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="G24">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H24">
-        <v>10.75</v>
+        <v>14</v>
       </c>
       <c r="I24">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J24">
+        <v>12.28</v>
+      </c>
+      <c r="K24">
+        <v>6.15</v>
+      </c>
+      <c r="L24">
+        <v>0.17</v>
+      </c>
+      <c r="M24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24">
+        <v>100</v>
+      </c>
+      <c r="O24">
         <v>200</v>
       </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>16</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>16</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1475,34 +1865,49 @@
         <v>2.9700000000000046</v>
       </c>
       <c r="F25">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="G25">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>10.75</v>
+        <v>17</v>
       </c>
       <c r="I25">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J25">
+        <v>12.28</v>
+      </c>
+      <c r="K25">
+        <v>6.15</v>
+      </c>
+      <c r="L25">
+        <v>0.17</v>
+      </c>
+      <c r="M25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25">
+        <v>100</v>
+      </c>
+      <c r="O25">
         <v>200</v>
       </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>16</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1517,34 +1922,49 @@
         <v>2.9400000000000048</v>
       </c>
       <c r="F26">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="G26">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H26">
-        <v>10.75</v>
+        <v>20</v>
       </c>
       <c r="I26">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J26">
+        <v>12.28</v>
+      </c>
+      <c r="K26">
+        <v>6.15</v>
+      </c>
+      <c r="L26">
+        <v>0.17</v>
+      </c>
+      <c r="M26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
+      <c r="O26">
         <v>200</v>
       </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1559,34 +1979,49 @@
         <v>2.910000000000005</v>
       </c>
       <c r="F27">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G27">
-        <v>0.81</v>
+        <v>5</v>
       </c>
       <c r="H27">
-        <v>10.75</v>
+        <v>23</v>
       </c>
       <c r="I27">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J27">
+        <v>12.28</v>
+      </c>
+      <c r="K27">
+        <v>6.15</v>
+      </c>
+      <c r="L27">
+        <v>0.17</v>
+      </c>
+      <c r="M27" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27">
         <v>200</v>
       </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>16</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1600,31 +2035,46 @@
         <f t="shared" si="0"/>
         <v>2.8800000000000052</v>
       </c>
-      <c r="F28">
-        <v>63</v>
+      <c r="F28" s="2">
+        <v>35</v>
       </c>
       <c r="G28">
-        <v>0.81</v>
-      </c>
-      <c r="H28">
-        <v>10.75</v>
+        <v>5</v>
+      </c>
+      <c r="H28" s="2">
+        <v>28</v>
       </c>
       <c r="I28">
-        <v>100</v>
+        <v>0.81</v>
       </c>
       <c r="J28">
+        <v>12.28</v>
+      </c>
+      <c r="K28">
+        <v>6.15</v>
+      </c>
+      <c r="L28">
+        <v>0.17</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
+      <c r="O28">
         <v>200</v>
       </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>16</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
         <v>0</v>
       </c>
     </row>

</xml_diff>